<commit_message>
chaprets 7 and 8 completed
</commit_message>
<xml_diff>
--- a/documentation.xlsx
+++ b/documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cordi\Desktop\SUMMA_PROJ\SummerProject2020DmitriiWeaver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389D5E8C-EC96-47FC-BF49-35E3C005A828}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC44B210-AF9B-4CCF-899E-735CCBC11FBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -59,9 +59,6 @@
     <t xml:space="preserve">chapter 3  and chapter 4 fully completed </t>
   </si>
   <si>
-    <t>chapter 4 was hard UwU</t>
-  </si>
-  <si>
     <t>freeday</t>
   </si>
   <si>
@@ -75,6 +72,21 @@
   </si>
   <si>
     <t>completed the exercises for chapter 6</t>
+  </si>
+  <si>
+    <t>red chapter 7 completedfirst exercise, stuck on the second</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chapter 4 was hard </t>
+  </si>
+  <si>
+    <t>internet died in the wholke area making it impossible to work</t>
+  </si>
+  <si>
+    <t>finished chapter 7</t>
+  </si>
+  <si>
+    <t>finished chapter 8</t>
   </si>
 </sst>
 </file>
@@ -396,7 +408,7 @@
   <dimension ref="A1:D90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -457,7 +469,7 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -467,8 +479,8 @@
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5" t="s">
-        <v>9</v>
+      <c r="D5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -479,7 +491,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -490,7 +502,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -501,7 +513,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -512,27 +524,51 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>43964</v>
       </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>43965</v>
       </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>43966</v>
       </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>43967</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
chapter 14 finished, docs filled
</commit_message>
<xml_diff>
--- a/documentation.xlsx
+++ b/documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cordi\Desktop\SUMMA_PROJ\SummerProject2020DmitriiWeaver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD84582-013F-428E-94B5-8DBA8117F46D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B63970F-5FEC-4BBC-9D9A-6A605FEBE599}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -114,6 +114,15 @@
   </si>
   <si>
     <t xml:space="preserve">had hard times working with the last exercise remembering about prototypes </t>
+  </si>
+  <si>
+    <t>short intro for HTML, good for revision</t>
+  </si>
+  <si>
+    <t>chapter 13 completed, chapter 14 red</t>
+  </si>
+  <si>
+    <t>chapter 14 completed, docs filled, github updated</t>
   </si>
 </sst>
 </file>
@@ -435,7 +444,7 @@
   <dimension ref="A1:D90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -680,15 +689,36 @@
       <c r="A20" s="1">
         <v>43974</v>
       </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>43975</v>
       </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>43976</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
chapters 15,16 and 17 completed
</commit_message>
<xml_diff>
--- a/documentation.xlsx
+++ b/documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cordi\Desktop\SUMMA_PROJ\SummerProject2020DmitriiWeaver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B63970F-5FEC-4BBC-9D9A-6A605FEBE599}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D030E8-A94C-49B1-A817-C1B63C94DE96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -123,6 +123,24 @@
   </si>
   <si>
     <t>chapter 14 completed, docs filled, github updated</t>
+  </si>
+  <si>
+    <t>chapter 15 completed</t>
+  </si>
+  <si>
+    <t>had to cheat on the third exercise as after 2.5 hours of work on the prev onesmy head simply did not work at all</t>
+  </si>
+  <si>
+    <t>studied chapter 16, completed first two exercises</t>
+  </si>
+  <si>
+    <t>had to look up some solutions as mine ones did not perform properly. Also had to look up some explainations on YT as the book did not give enough info</t>
+  </si>
+  <si>
+    <t>finished chapter 16</t>
+  </si>
+  <si>
+    <t>chapter 17 completed</t>
   </si>
 </sst>
 </file>
@@ -443,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,7 +470,7 @@
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="24.88671875" customWidth="1"/>
     <col min="3" max="3" width="47.5546875" customWidth="1"/>
-    <col min="4" max="4" width="112" customWidth="1"/>
+    <col min="4" max="4" width="116.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -725,25 +743,61 @@
       <c r="A23" s="1">
         <v>43977</v>
       </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>43978</v>
       </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>43979</v>
       </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>43980</v>
       </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>43981</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
chapter 18 exercises 1 and 2
</commit_message>
<xml_diff>
--- a/documentation.xlsx
+++ b/documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cordi\Desktop\SUMMA_PROJ\SummerProject2020DmitriiWeaver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D030E8-A94C-49B1-A817-C1B63C94DE96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA2D353-EA4D-4E89-BE94-D4EADDC30970}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t>chapter 17 completed</t>
+  </si>
+  <si>
+    <t>chapter 18 red, exercises 1 and 2 completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> freeday due to doctors appointment</t>
   </si>
 </sst>
 </file>
@@ -461,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -804,15 +810,33 @@
       <c r="A28" s="1">
         <v>43982</v>
       </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>43983</v>
       </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="D29" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>43984</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="D30" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
lots of things added
</commit_message>
<xml_diff>
--- a/documentation.xlsx
+++ b/documentation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cordi\Desktop\SUMMA_PROJ\SummerProject2020DmitriiWeaver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA2D353-EA4D-4E89-BE94-D4EADDC30970}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0478628-E3E5-419D-8290-EDA097E06250}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
   <si>
     <t>Date</t>
   </si>
@@ -147,6 +147,48 @@
   </si>
   <si>
     <t xml:space="preserve"> freeday due to doctors appointment</t>
+  </si>
+  <si>
+    <t>studied chapter 19</t>
+  </si>
+  <si>
+    <t>another doctors appointment</t>
+  </si>
+  <si>
+    <t>additional research via YT and w3schools</t>
+  </si>
+  <si>
+    <t>started working on chapter 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">revising </t>
+  </si>
+  <si>
+    <t>looked up the game project in the book to get some concepts for the practical part</t>
+  </si>
+  <si>
+    <t>freeday, was moving back to Oulu</t>
+  </si>
+  <si>
+    <t>freeday was moving from Oulu</t>
+  </si>
+  <si>
+    <t>documentation work, reorganising working schedule, revision</t>
+  </si>
+  <si>
+    <t>additional studying of parcers based on prev exercises</t>
+  </si>
+  <si>
+    <t>almost finished chapter 20</t>
+  </si>
+  <si>
+    <t>node programming goes very hard</t>
+  </si>
+  <si>
+    <t>still  very confused with node coding, ned more info</t>
+  </si>
+  <si>
+    <t>node still does not work well</t>
   </si>
 </sst>
 </file>
@@ -467,15 +509,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="B23" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="24.88671875" customWidth="1"/>
-    <col min="3" max="3" width="47.5546875" customWidth="1"/>
+    <col min="3" max="3" width="50.33203125" customWidth="1"/>
     <col min="4" max="4" width="116.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -843,88 +885,184 @@
       <c r="A31" s="1">
         <v>43985</v>
       </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>43986</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="D32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>43987</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>43988</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>43989</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="D35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>43990</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="D36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>43991</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>43992</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>43993</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="D39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>43994</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>43995</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>43996</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="D42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>43997</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="D43" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>43998</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
+        <v>46</v>
+      </c>
+      <c r="D44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>43999</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>44000</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>44001</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>44002</v>
       </c>

</xml_diff>

<commit_message>
game made more presentable
</commit_message>
<xml_diff>
--- a/documentation.xlsx
+++ b/documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cordi\Desktop\SUMMA_PROJ\SummerProject2020DmitriiWeaver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AC7842-2989-412F-962C-1BFFE6FBAD33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52BCE91B-1DB0-452E-84A3-55B3C111D451}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
   <si>
     <t>Date</t>
   </si>
@@ -234,6 +234,9 @@
   </si>
   <si>
     <t>entity interactions added</t>
+  </si>
+  <si>
+    <t>refactoring, making the game look more presentable</t>
   </si>
 </sst>
 </file>
@@ -555,7 +558,7 @@
   <dimension ref="A1:D90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1264,6 +1267,12 @@
       <c r="A60" s="1">
         <v>44014</v>
       </c>
+      <c r="B60">
+        <v>3</v>
+      </c>
+      <c r="C60" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1">

</xml_diff>

<commit_message>
music added, some experiments made
</commit_message>
<xml_diff>
--- a/documentation.xlsx
+++ b/documentation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cordi\Desktop\SUMMA_PROJ\SummerProject2020DmitriiWeaver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042B96A6-A37E-446C-9627-96BF41B21256}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806D621F-C031-4ECA-8E00-212146538643}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="75">
   <si>
     <t>Date</t>
   </si>
@@ -249,6 +249,15 @@
   </si>
   <si>
     <t>new enemy added, some refactoring done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">refactoring done, added interaction with tiles by a player </t>
+  </si>
+  <si>
+    <t>basically an ability to delete or "break" tiles from inside of the game</t>
+  </si>
+  <si>
+    <t xml:space="preserve">added music, experimented more with replacing variables, textures and sounds </t>
   </si>
 </sst>
 </file>
@@ -569,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B51" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" topLeftCell="B45" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1356,10 +1365,25 @@
       <c r="A67" s="1">
         <v>44021</v>
       </c>
+      <c r="B67">
+        <v>8</v>
+      </c>
+      <c r="C67" t="s">
+        <v>72</v>
+      </c>
+      <c r="D67" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>44022</v>
+      </c>
+      <c r="B68">
+        <v>5</v>
+      </c>
+      <c r="C68" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
music control added, refactoring done
</commit_message>
<xml_diff>
--- a/documentation.xlsx
+++ b/documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cordi\Desktop\SUMMA_PROJ\SummerProject2020DmitriiWeaver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E19AA835-3EBD-40F7-8F6E-195B191794C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5635BDA4-9FED-4D21-8483-AE91248A2142}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="77">
   <si>
     <t>Date</t>
   </si>
@@ -261,6 +261,9 @@
   </si>
   <si>
     <t>refactoring, fixing old bugs and the bugs created while fixing old ones</t>
+  </si>
+  <si>
+    <t>music control, fixing bugs MORE REFACTORING</t>
   </si>
 </sst>
 </file>
@@ -582,7 +585,7 @@
   <dimension ref="A1:D90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1415,6 +1418,12 @@
       <c r="A71" s="1">
         <v>44025</v>
       </c>
+      <c r="B71">
+        <v>6</v>
+      </c>
+      <c r="C71" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1">

</xml_diff>

<commit_message>
started building level progression
</commit_message>
<xml_diff>
--- a/documentation.xlsx
+++ b/documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cordi\Desktop\SUMMA_PROJ\SummerProject2020DmitriiWeaver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51B0F35-0728-4EE4-A01A-7516A361EC24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C9570C-8DA9-446F-9806-F778094DCDCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="79">
   <si>
     <t>Date</t>
   </si>
@@ -267,6 +267,9 @@
   </si>
   <si>
     <t>coins added</t>
+  </si>
+  <si>
+    <t>started building level progression, refactored even more things</t>
   </si>
 </sst>
 </file>
@@ -587,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B49" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1454,6 +1457,12 @@
       <c r="A74" s="1">
         <v>44028</v>
       </c>
+      <c r="B74">
+        <v>7</v>
+      </c>
+      <c r="C74" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1">

</xml_diff>

<commit_message>
attempt to fix bugs
</commit_message>
<xml_diff>
--- a/documentation.xlsx
+++ b/documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cordi\Desktop\SUMMA_PROJ\SummerProject2020DmitriiWeaver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606FA8A4-785B-46B5-AB16-B3B65C7FBE1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B128C5D-1FCF-4D70-B850-D23A0FC27B37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="83">
   <si>
     <t>Date</t>
   </si>
@@ -279,6 +279,9 @@
   </si>
   <si>
     <t>refactoring, fixing bugs</t>
+  </si>
+  <si>
+    <t>attempts to fix bugs, side studying</t>
   </si>
 </sst>
 </file>
@@ -600,7 +603,7 @@
   <dimension ref="A1:D90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B55" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1521,6 +1524,12 @@
       <c r="A79" s="1">
         <v>44033</v>
       </c>
+      <c r="B79">
+        <v>6</v>
+      </c>
+      <c r="C79" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1">

</xml_diff>

<commit_message>
some bug fixes + graphics rebuild
</commit_message>
<xml_diff>
--- a/documentation.xlsx
+++ b/documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cordi\Desktop\SUMMA_PROJ\SummerProject2020DmitriiWeaver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B128C5D-1FCF-4D70-B850-D23A0FC27B37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99EAD71-17E1-443E-9153-D44D26673FEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="85">
   <si>
     <t>Date</t>
   </si>
@@ -282,6 +282,12 @@
   </si>
   <si>
     <t>attempts to fix bugs, side studying</t>
+  </si>
+  <si>
+    <t>level design</t>
+  </si>
+  <si>
+    <t>bugs fixed, other bugs added, tiles redraw</t>
   </si>
 </sst>
 </file>
@@ -602,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B55" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1535,53 +1541,65 @@
       <c r="A80" s="1">
         <v>44034</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B80">
+        <v>7</v>
+      </c>
+      <c r="C80" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>44035</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B81">
+        <v>6</v>
+      </c>
+      <c r="C81" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>44036</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>44037</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>44038</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>44039</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>44040</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>44041</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>44042</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>44043</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>44044</v>
       </c>

</xml_diff>